<commit_message>
Versión final de CS_06_01_CO sin .mm
Versión final guion sin mapa conceptual + lo que llevo de CS_06_04_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion01/EsqueletoGuion_CS_06_01_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion01/EsqueletoGuion_CS_06_01_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="13125" tabRatio="729" activeTab="1"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="13125" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -13,20 +13,20 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="85">
   <si>
     <t>FICHA</t>
   </si>
@@ -275,6 +275,12 @@
   </si>
   <si>
     <t>Asocia cada tipo de escritura a su soporte</t>
+  </si>
+  <si>
+    <t>Competencias</t>
+  </si>
+  <si>
+    <t>Comprende cómo se realiza la definición de fechas y edades</t>
   </si>
 </sst>
 </file>
@@ -1505,7 +1511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1578,8 +1584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,7 +2100,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D30"/>
@@ -2436,22 +2442,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="52.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.140625" customWidth="1"/>
+    <col min="8" max="8" width="59.140625" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2582,32 +2588,34 @@
         <v>48</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>53</v>
-      </c>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+        <v>74</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="5"/>
+      <c r="H8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2617,18 +2625,13 @@
         <v>50</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2638,16 +2641,13 @@
         <v>50</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="5" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2657,15 +2657,13 @@
         <v>50</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2675,7 +2673,17 @@
         <v>50</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2686,7 +2694,13 @@
         <v>50</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>45</v>
+        <v>51</v>
+      </c>
+      <c r="H13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2696,18 +2710,11 @@
       <c r="B14" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2716,32 +2723,29 @@
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="5"/>
@@ -2751,18 +2755,23 @@
         <v>19</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="8" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
-      <c r="H17" s="5"/>
+      <c r="H17" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -2771,17 +2780,13 @@
       <c r="B18" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8" t="s">
-        <v>55</v>
-      </c>
+      <c r="C18" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="8"/>
       <c r="E18" s="8"/>
-      <c r="F18" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>45</v>
-      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2795,13 +2800,11 @@
       <c r="D19" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="8" t="s">
+      <c r="E19" s="8" t="s">
         <v>45</v>
       </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2815,13 +2818,14 @@
       <c r="D20" s="8" t="s">
         <v>55</v>
       </c>
+      <c r="E20" s="8"/>
       <c r="F20" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I20" s="8"/>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -2834,12 +2838,14 @@
       <c r="D21" s="8" t="s">
         <v>55</v>
       </c>
+      <c r="E21" s="8"/>
       <c r="F21" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>62</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2852,14 +2858,13 @@
       <c r="D22" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="8"/>
       <c r="F22" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H22" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -2870,14 +2875,14 @@
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -2888,13 +2893,15 @@
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+        <v>55</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2906,7 +2913,7 @@
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>45</v>
@@ -2922,12 +2929,16 @@
       <c r="B26" s="7" t="s">
         <v>54</v>
       </c>
+      <c r="C26" s="7"/>
       <c r="D26" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>62</v>
       </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -2936,12 +2947,16 @@
       <c r="B27" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="C27" s="7"/>
+      <c r="D27" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="8" t="s">
         <v>45</v>
       </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -2950,8 +2965,8 @@
       <c r="B28" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>61</v>
+      <c r="D28" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>62</v>
@@ -2968,7 +2983,7 @@
         <v>61</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2979,10 +2994,10 @@
         <v>54</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2993,7 +3008,7 @@
         <v>54</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>62</v>
@@ -3010,7 +3025,7 @@
         <v>64</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3024,7 +3039,7 @@
         <v>64</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3038,7 +3053,7 @@
         <v>64</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -3052,13 +3067,7 @@
         <v>64</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -3072,13 +3081,7 @@
         <v>64</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -3089,15 +3092,15 @@
         <v>54</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H37" t="s">
-        <v>28</v>
-      </c>
-      <c r="I37" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I37" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3106,10 +3109,19 @@
         <v>19</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -3117,26 +3129,34 @@
         <v>19</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H39" s="9"/>
+      <c r="I39" s="8"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I40" s="5" t="s">
+      <c r="H40" t="s">
+        <v>28</v>
+      </c>
+      <c r="I40" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3147,10 +3167,7 @@
       <c r="B41" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3161,11 +3178,8 @@
       <c r="B42" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>62</v>
+      <c r="C42" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3175,14 +3189,11 @@
       <c r="B43" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>51</v>
+      <c r="C43" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>43</v>
@@ -3196,7 +3207,7 @@
         <v>65</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>45</v>
@@ -3210,7 +3221,7 @@
         <v>65</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>62</v>
@@ -3224,13 +3235,13 @@
         <v>65</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>51</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I46" s="5" t="s">
         <v>43</v>
@@ -3247,13 +3258,7 @@
         <v>31</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -3264,10 +3269,10 @@
         <v>65</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3278,10 +3283,16 @@
         <v>65</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>62</v>
+        <v>51</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -3292,13 +3303,13 @@
         <v>65</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H50" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I50" s="5" t="s">
         <v>43</v>
@@ -3312,7 +3323,7 @@
         <v>65</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>45</v>
@@ -3326,10 +3337,10 @@
         <v>65</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -3340,10 +3351,16 @@
         <v>65</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -3357,13 +3374,7 @@
         <v>34</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3377,13 +3388,7 @@
         <v>34</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H55" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3394,16 +3399,10 @@
         <v>65</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H56" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I56" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3411,81 +3410,85 @@
         <v>19</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>45</v>
+        <v>65</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>66</v>
+      <c r="B58" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>19</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>66</v>
+      <c r="B59" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G59" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="H59" s="9"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>19</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>66</v>
+      <c r="B60" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>62</v>
+        <v>48</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I60" s="8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>19</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H61" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="I61" s="5" t="s">
-        <v>43</v>
+      <c r="C61" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3496,7 +3499,7 @@
         <v>66</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>45</v>
@@ -3510,10 +3513,13 @@
         <v>66</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3524,16 +3530,13 @@
         <v>66</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H64" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I64" s="8" t="s">
-        <v>43</v>
+        <v>67</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3544,15 +3547,18 @@
         <v>66</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E65" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G65" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H65" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I65" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I65" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3561,16 +3567,13 @@
         <v>19</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H66" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I66" s="5" t="s">
-        <v>43</v>
+        <v>66</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3578,16 +3581,13 @@
         <v>19</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H67" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I67" s="5" t="s">
-        <v>43</v>
+        <v>66</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3595,15 +3595,18 @@
         <v>19</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>41</v>
+        <v>66</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="H68" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I68" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I68" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3612,16 +3615,103 @@
         <v>19</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H69" s="9"/>
+      <c r="I69" s="8"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H70" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I70" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H71" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H72" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I72" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C73" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>19</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H69" s="9" t="s">
+      <c r="H74" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I69" s="5" t="s">
-        <v>43</v>
+      <c r="I74" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CS0601: Ajuste de errores de nombres
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion01/EsqueletoGuion_CS_06_01_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion01/EsqueletoGuion_CS_06_01_CO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\CienciasSociales\fuentes\contenidos\grado06\guion01\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23240" windowHeight="19900" tabRatio="729"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23244" windowHeight="19904" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -13,20 +18,20 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="83">
   <si>
     <t>FICHA</t>
   </si>
@@ -133,9 +138,6 @@
     <t>Las fuentes escritas</t>
   </si>
   <si>
-    <t xml:space="preserve">Asocia cada tipo de escritura al soporte </t>
-  </si>
-  <si>
     <t>Reconoce tipos de restos arqueológicos</t>
   </si>
   <si>
@@ -272,9 +274,6 @@
   </si>
   <si>
     <t>Competencias</t>
-  </si>
-  <si>
-    <t>Comprende cómo se realiza la definición de fechas y edades</t>
   </si>
   <si>
     <t>no</t>
@@ -1542,7 +1541,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1556,13 +1555,13 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="1" max="1" width="22.46484375" customWidth="1"/>
     <col min="2" max="2" width="104.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
@@ -1570,7 +1569,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
@@ -1578,23 +1577,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
         <v>1</v>
       </c>
@@ -1602,7 +1601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
@@ -1626,22 +1625,22 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.33203125" customWidth="1"/>
-    <col min="4" max="4" width="68.1640625" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="68.1328125" customWidth="1"/>
+    <col min="5" max="5" width="20.46484375" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15">
+    <row r="1" spans="1:14" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -1661,21 +1660,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="4" customFormat="1">
+    <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
         <v>73</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>74</v>
-      </c>
-      <c r="C2" t="s">
-        <v>75</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -1689,361 +1688,361 @@
       <c r="M2"/>
       <c r="N2"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
         <v>73</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>74</v>
-      </c>
-      <c r="C3" t="s">
-        <v>75</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
       </c>
       <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
         <v>78</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>79</v>
       </c>
       <c r="F4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
         <v>73</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>74</v>
-      </c>
-      <c r="C5" t="s">
-        <v>75</v>
       </c>
       <c r="D5" t="s">
         <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
         <v>73</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>74</v>
-      </c>
-      <c r="C6" t="s">
-        <v>75</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
         <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
         <v>73</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>74</v>
-      </c>
-      <c r="C9" t="s">
-        <v>75</v>
       </c>
       <c r="D9" t="s">
         <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
         <v>73</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>74</v>
-      </c>
-      <c r="C10" t="s">
-        <v>75</v>
       </c>
       <c r="D10" t="s">
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
         <v>73</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>74</v>
-      </c>
-      <c r="C11" t="s">
-        <v>75</v>
       </c>
       <c r="D11" t="s">
         <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F11">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
         <v>73</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>74</v>
-      </c>
-      <c r="C12" t="s">
-        <v>75</v>
       </c>
       <c r="D12" t="s">
         <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F12">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
         <v>73</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>74</v>
-      </c>
-      <c r="C13" t="s">
-        <v>75</v>
       </c>
       <c r="D13" t="s">
         <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F13">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" t="s">
         <v>73</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>74</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" t="s">
         <v>75</v>
-      </c>
-      <c r="D14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" t="s">
-        <v>76</v>
       </c>
       <c r="F14">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" t="s">
         <v>73</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>74</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
         <v>75</v>
-      </c>
-      <c r="D15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" t="s">
-        <v>76</v>
       </c>
       <c r="F15">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
         <v>73</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>74</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
         <v>75</v>
-      </c>
-      <c r="D16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" t="s">
-        <v>76</v>
       </c>
       <c r="F16">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" t="s">
         <v>73</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>74</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
         <v>75</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" t="s">
-        <v>76</v>
       </c>
       <c r="F17">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" t="s">
         <v>73</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>74</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
         <v>75</v>
-      </c>
-      <c r="D18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" t="s">
-        <v>76</v>
       </c>
       <c r="F18">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
         <v>73</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>74</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
         <v>75</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" t="s">
         <v>39</v>
       </c>
-      <c r="E19" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>75</v>
-      </c>
-      <c r="D20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" t="s">
-        <v>76</v>
       </c>
       <c r="F20">
         <v>20</v>
@@ -2068,13 +2067,13 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="66.1640625" customWidth="1"/>
+    <col min="1" max="1" width="66.1328125" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
@@ -2085,43 +2084,43 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1">
+    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="15"/>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1">
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C3" s="2">
         <v>21</v>
       </c>
       <c r="D3" s="15"/>
     </row>
-    <row r="4" spans="1:4" s="4" customFormat="1">
+    <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="29" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4" s="29">
         <v>22</v>
       </c>
       <c r="D4" s="15"/>
     </row>
-    <row r="5" spans="1:4" s="4" customFormat="1">
+    <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
     </row>
@@ -2141,23 +2140,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C23" sqref="A23:C23"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="92.33203125" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
@@ -2168,7 +2167,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -2176,11 +2175,11 @@
         <v>19</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D2" s="15"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -2188,11 +2187,11 @@
         <v>23</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D3" s="15"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -2200,23 +2199,23 @@
         <v>24</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D4" s="15"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="15">
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D5" s="15"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -2224,11 +2223,11 @@
         <v>26</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D6" s="15"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -2236,11 +2235,11 @@
         <v>27</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D7" s="15"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -2248,11 +2247,11 @@
         <v>28</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -2260,11 +2259,11 @@
         <v>29</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D9" s="15"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="15">
         <v>9</v>
       </c>
@@ -2272,11 +2271,11 @@
         <v>30</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D10" s="15"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -2284,11 +2283,11 @@
         <v>31</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D11" s="15"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="15">
         <v>11</v>
       </c>
@@ -2296,11 +2295,11 @@
         <v>32</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D12" s="15"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -2308,11 +2307,11 @@
         <v>33</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D13" s="15"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -2320,107 +2319,107 @@
         <v>34</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D14" s="15"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="15">
         <v>14</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D15" s="15"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="15">
         <v>15</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D16" s="15"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="15">
         <v>16</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D17" s="15"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="15">
         <v>17</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D18" s="15"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="15">
         <v>18</v>
       </c>
       <c r="B19" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="15">
+        <v>19</v>
+      </c>
+      <c r="B20" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="15"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="15">
-        <v>19</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>39</v>
-      </c>
       <c r="C20" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D20" s="15"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="15">
         <v>20</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D21" s="15"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="15">
         <v>21</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D22" s="15"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="29">
         <v>22</v>
       </c>
@@ -2428,41 +2427,41 @@
         <v>25</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D23" s="15"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="15"/>
       <c r="B24" s="16"/>
       <c r="C24" s="17"/>
       <c r="D24" s="15"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
       <c r="C25" s="17"/>
       <c r="D25" s="15"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
       <c r="C26" s="17"/>
       <c r="D26" s="15"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B27" s="4"/>
       <c r="C27" s="18"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B28" s="4"/>
       <c r="C28" s="19"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B29" s="4"/>
       <c r="C29" s="19"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B30" s="4"/>
       <c r="C30" s="19"/>
     </row>
@@ -2485,24 +2484,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+    <sheetView topLeftCell="D34" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="40.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="40.46484375" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="52.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="31.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="59.1640625" customWidth="1"/>
-    <col min="9" max="9" width="17.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.1328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.796875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="31.46484375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.796875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="59.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.46484375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15">
+    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
@@ -2531,15 +2530,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
@@ -2548,15 +2547,15 @@
       <c r="H2" s="25"/>
       <c r="I2" s="25"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
@@ -2565,95 +2564,95 @@
       <c r="H3" s="25"/>
       <c r="I3" s="25"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="24"/>
       <c r="G4" s="24"/>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" s="24"/>
       <c r="G5" s="24"/>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>45</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>46</v>
       </c>
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="24" t="s">
         <v>47</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>48</v>
       </c>
       <c r="F8" s="24"/>
       <c r="G8" s="24"/>
@@ -2661,18 +2660,18 @@
         <v>19</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -2680,15 +2679,15 @@
       <c r="G9" s="8"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -2696,15 +2695,15 @@
       <c r="G10" s="8"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -2712,15 +2711,15 @@
       <c r="G11" s="8"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -2730,105 +2729,105 @@
         <v>23</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="H13" t="s">
         <v>24</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>48</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
@@ -2837,371 +2836,371 @@
       <c r="H18" s="25"/>
       <c r="I18" s="25"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F19" s="24"/>
       <c r="G19" s="24"/>
       <c r="H19" s="25"/>
       <c r="I19" s="25"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="23"/>
       <c r="D20" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20" s="24"/>
       <c r="F20" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H20" s="25"/>
       <c r="I20" s="25"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="24"/>
       <c r="F21" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H21" s="25"/>
       <c r="I21" s="25"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="23"/>
       <c r="D22" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E22" s="26"/>
       <c r="F22" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H22" s="22"/>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E23" s="26"/>
       <c r="F23" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H23" s="22"/>
       <c r="I23" s="25"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" s="23"/>
       <c r="D24" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E24" s="24"/>
       <c r="F24" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H24" s="25"/>
       <c r="I24" s="25"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25" s="24"/>
       <c r="H25" s="25"/>
       <c r="I25" s="25"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="23"/>
       <c r="D26" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F26" s="24"/>
       <c r="G26" s="24"/>
       <c r="H26" s="25"/>
       <c r="I26" s="25"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" s="23"/>
       <c r="D27" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
       <c r="H27" s="25"/>
       <c r="I27" s="25"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F28" s="26"/>
       <c r="G28" s="26"/>
       <c r="H28" s="22"/>
       <c r="I28" s="25"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="27"/>
       <c r="D29" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F29" s="26"/>
       <c r="G29" s="26"/>
       <c r="H29" s="22"/>
       <c r="I29" s="25"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="27"/>
       <c r="D30" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="26" t="s">
         <v>59</v>
-      </c>
-      <c r="E30" s="26" t="s">
-        <v>60</v>
       </c>
       <c r="F30" s="26"/>
       <c r="G30" s="26"/>
       <c r="H30" s="22"/>
       <c r="I30" s="25"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C31" s="27"/>
       <c r="D31" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="26" t="s">
         <v>59</v>
-      </c>
-      <c r="E31" s="26" t="s">
-        <v>60</v>
       </c>
       <c r="F31" s="26"/>
       <c r="G31" s="26"/>
       <c r="H31" s="22"/>
       <c r="I31" s="25"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C32" s="27"/>
       <c r="D32" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F32" s="26"/>
       <c r="G32" s="26"/>
       <c r="H32" s="22"/>
       <c r="I32" s="25"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C33" s="27"/>
       <c r="D33" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E33" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F33" s="26"/>
       <c r="G33" s="26"/>
       <c r="H33" s="22"/>
       <c r="I33" s="25"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C34" s="27"/>
       <c r="D34" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F34" s="26"/>
       <c r="G34" s="26"/>
       <c r="H34" s="22"/>
       <c r="I34" s="25"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C35" s="27"/>
       <c r="D35" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F35" s="26"/>
       <c r="G35" s="26"/>
       <c r="H35" s="22"/>
       <c r="I35" s="25"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" s="27"/>
       <c r="D36" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F36" s="26"/>
       <c r="G36" s="26"/>
       <c r="H36" s="22"/>
       <c r="I36" s="25"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="27"/>
       <c r="D37" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F37" s="26"/>
       <c r="G37" s="26"/>
@@ -3209,22 +3208,22 @@
         <v>26</v>
       </c>
       <c r="I37" s="24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C38" s="27"/>
       <c r="D38" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F38" s="26"/>
       <c r="G38" s="26"/>
@@ -3232,41 +3231,41 @@
         <v>27</v>
       </c>
       <c r="I38" s="24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C39" s="27"/>
       <c r="D39" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F39" s="26"/>
       <c r="G39" s="26"/>
       <c r="H39" s="28"/>
       <c r="I39" s="24"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C40" s="27"/>
       <c r="D40" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E40" s="26" t="s">
         <v>47</v>
-      </c>
-      <c r="E40" s="26" t="s">
-        <v>48</v>
       </c>
       <c r="F40" s="26"/>
       <c r="G40" s="26"/>
@@ -3274,338 +3273,338 @@
         <v>28</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>19</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>19</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H43" s="9" t="s">
         <v>29</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>19</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>19</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H46" s="9" t="s">
         <v>30</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>19</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>19</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>19</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H49" s="9" t="s">
         <v>31</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>19</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H50" s="9" t="s">
         <v>32</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>19</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>19</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H53" s="9" t="s">
         <v>33</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>19</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>19</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>19</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H57" s="9" t="s">
         <v>34</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>19</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H58" s="9" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>19</v>
       </c>
       <c r="B59" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H59" s="9"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A61" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H59" s="9"/>
-    </row>
-    <row r="60" spans="1:9">
-      <c r="A60" t="s">
-        <v>19</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H60" s="9" t="s">
+      <c r="C61" s="27" t="s">
         <v>43</v>
-      </c>
-      <c r="I60" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B61" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="C61" s="27" t="s">
-        <v>44</v>
       </c>
       <c r="D61" s="26"/>
       <c r="E61" s="26"/>
@@ -3614,252 +3613,252 @@
       <c r="H61" s="22"/>
       <c r="I61" s="25"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B62" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C62" s="27"/>
       <c r="D62" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E62" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F62" s="26"/>
       <c r="G62" s="26"/>
       <c r="H62" s="22"/>
       <c r="I62" s="25"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B63" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C63" s="27"/>
       <c r="D63" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E63" s="26"/>
       <c r="F63" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G63" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H63" s="22"/>
       <c r="I63" s="25"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B64" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C64" s="27"/>
       <c r="D64" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E64" s="26"/>
       <c r="F64" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G64" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H64" s="22"/>
       <c r="I64" s="25"/>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B65" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C65" s="27"/>
       <c r="D65" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E65" s="26"/>
       <c r="F65" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G65" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H65" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I65" s="24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B66" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C66" s="27"/>
       <c r="D66" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E66" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F66" s="26"/>
       <c r="G66" s="26"/>
       <c r="H66" s="22"/>
       <c r="I66" s="25"/>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B67" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C67" s="27"/>
       <c r="D67" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E67" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F67" s="26"/>
       <c r="G67" s="26"/>
       <c r="H67" s="22"/>
       <c r="I67" s="25"/>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B68" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C68" s="27"/>
       <c r="D68" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E68" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F68" s="26"/>
       <c r="G68" s="26"/>
       <c r="H68" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I68" s="24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B69" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C69" s="27"/>
       <c r="D69" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E69" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F69" s="26"/>
       <c r="G69" s="26"/>
       <c r="H69" s="28"/>
       <c r="I69" s="24"/>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B70" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C70" s="27"/>
       <c r="D70" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E70" s="26" t="s">
         <v>47</v>
-      </c>
-      <c r="E70" s="26" t="s">
-        <v>48</v>
       </c>
       <c r="F70" s="26"/>
       <c r="G70" s="26"/>
       <c r="H70" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="I70" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H71" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="I70" s="24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
-      <c r="A71" t="s">
-        <v>19</v>
-      </c>
-      <c r="B71" s="2" t="s">
+      <c r="I71" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H72" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I72" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I73" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H71" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I71" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
-      <c r="A72" t="s">
-        <v>19</v>
-      </c>
-      <c r="B72" s="2" t="s">
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A74" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B74" s="29" t="s">
         <v>68</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H72" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I72" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
-      <c r="A73" t="s">
-        <v>19</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H73" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I73" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
-      <c r="A74" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B74" s="29" t="s">
-        <v>69</v>
       </c>
       <c r="C74" s="29" t="s">
         <v>25</v>
@@ -3872,7 +3871,7 @@
         <v>25</v>
       </c>
       <c r="I74" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>